<commit_message>
Updated output file example for querying.
</commit_message>
<xml_diff>
--- a/tblLocation/validation_result.xlsx
+++ b/tblLocation/validation_result.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>Index</t>
   </si>
@@ -50,22 +50,82 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Kilombo Experimental Station, Angola</t>
-  </si>
-  <si>
-    <t>Angola</t>
-  </si>
-  <si>
-    <t>AGO</t>
-  </si>
-  <si>
-    <t>Kilombo Experimental Station</t>
+    <t>Darul Aman Kabul (2), Afghanistan</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>AFG</t>
+  </si>
+  <si>
+    <t>Darul Aman Kabul (2)</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>correct location data</t>
+  </si>
+  <si>
+    <t>Dinajpur, 5216, Rangpur Division, Bangladesh</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>BGD</t>
+  </si>
+  <si>
+    <t>Dinajpur</t>
+  </si>
+  <si>
+    <t>no lat/lng entered / incorrect lat/lng - geocoded location</t>
+  </si>
+  <si>
+    <t>Bolivia, Plurinational State of</t>
+  </si>
+  <si>
+    <t>BOL</t>
+  </si>
+  <si>
+    <t>Lomas De Arena (santa Cruz)</t>
+  </si>
+  <si>
+    <t>South America</t>
+  </si>
+  <si>
+    <t>incorrect location data/cannot find coordinates</t>
+  </si>
+  <si>
+    <t>Zamseed, Farm, Zambia</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>ZMB</t>
+  </si>
+  <si>
+    <t>Zamseed, Farm</t>
   </si>
   <si>
     <t>Eastern and Southern Africa</t>
   </si>
   <si>
-    <t>correct location data</t>
+    <t>Guadalajara, 44100, Jalisco, Mexico</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>MEX</t>
+  </si>
+  <si>
+    <t>Guadalajara, Jalisco</t>
+  </si>
+  <si>
+    <t>Central America and Caribbean</t>
   </si>
 </sst>
 </file>
@@ -414,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,7 +519,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -471,25 +531,159 @@
         <v>13</v>
       </c>
       <c r="E2" t="n">
-        <v>-8.9</v>
+        <v>34.48845</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
       </c>
       <c r="G2" t="n">
-        <v>14.7</v>
+        <v>69.20287999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>-8.9</v>
+        <v>34.48845</v>
       </c>
       <c r="I2" t="n">
-        <v>14.7</v>
+        <v>69.20287999999999</v>
       </c>
       <c r="J2" t="s">
         <v>15</v>
       </c>
       <c r="K2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>25.6260712</v>
+      </c>
+      <c r="I3" t="n">
+        <v>88.6346228</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s"/>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s"/>
+      <c r="I4" t="s"/>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-14.2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="n">
+        <v>28.4</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-14.2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>28.4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="n">
+        <v>599</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>20.676143</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-103.3469982</v>
+      </c>
+      <c r="J6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>